<commit_message>
21 march Turkey data
</commit_message>
<xml_diff>
--- a/Korona/data/vaka_sayisi_tur.xlsx
+++ b/Korona/data/vaka_sayisi_tur.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serda\Documents\workingdirectory\shiny-server\Korona\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B5F78D-7EEE-4C1C-A97A-6464FE49CD65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CDE357-743A-40E3-9689-7534914D838A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="200" windowWidth="19200" windowHeight="10050" xr2:uid="{407975B0-CCB0-40CD-90AE-1021614F5B8C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{407975B0-CCB0-40CD-90AE-1021614F5B8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Turkiye</t>
   </si>
@@ -54,6 +55,15 @@
   </si>
   <si>
     <t>olen</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>tested</t>
+  </si>
+  <si>
+    <t>percent_pos</t>
   </si>
 </sst>
 </file>
@@ -418,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B42DD3-910F-4F01-92FC-89DC173690B5}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,8 +659,73 @@
         <v>661</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43911</v>
+      </c>
+      <c r="D12" s="2">
+        <v>947</v>
+      </c>
+      <c r="E12">
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <f>D12-E12</f>
+        <v>926</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46DE464-F485-4042-8655-CD20F51E3B9C}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>43910</v>
+      </c>
+      <c r="B2">
+        <v>3656</v>
+      </c>
+      <c r="C2">
+        <v>311</v>
+      </c>
+      <c r="D2">
+        <f>C2/B2*100</f>
+        <v>8.5065645514223203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modify to fit new JHU sheet
</commit_message>
<xml_diff>
--- a/Korona/data/vaka_sayisi_tur.xlsx
+++ b/Korona/data/vaka_sayisi_tur.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serda\Documents\workingdirectory\shiny-server\Korona\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D4627B-0EDF-4320-A148-D00862602D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002F3C6F-CBDF-4314-9C5D-D60E365DC4A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{407975B0-CCB0-40CD-90AE-1021614F5B8C}"/>
+    <workbookView xWindow="8676" yWindow="600" windowWidth="30960" windowHeight="15852" xr2:uid="{407975B0-CCB0-40CD-90AE-1021614F5B8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -449,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B42DD3-910F-4F01-92FC-89DC173690B5}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,6 +720,21 @@
       <c r="F13">
         <f>D13-E13</f>
         <v>1206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1539</v>
+      </c>
+      <c r="E14">
+        <v>37</v>
+      </c>
+      <c r="F14">
+        <f>D14-E14</f>
+        <v>1502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>